<commit_message>
finished with js and webpacker, active job, active storage. fixed some styles, as well as flash messages. started working with mailers
</commit_message>
<xml_diff>
--- a/bookings_report.xlsx
+++ b/bookings_report.xlsx
@@ -370,7 +370,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetData>
     <row r="1" spans="1:4" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -526,6 +526,48 @@
         <v>2022-10-09 21:50:26 UTC</v>
       </c>
     </row>
+    <row r="12" spans="1:4" customFormat="false">
+      <c r="A12" s="0" t="str">
+        <v>gh</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <v>eroha@gmail.com</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <v>2022-10-10 00:00:00 UTC</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <v>2022-10-13 00:00:00 UTC</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" customFormat="false">
+      <c r="A13" s="0" t="str">
+        <v>name</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <v>email@email.com</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <v>2022-10-16 00:00:00 UTC</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <v>2022-10-17 00:00:00 UTC</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" customFormat="false">
+      <c r="A14" s="0" t="str">
+        <v>Ivan Knyazev</v>
+      </c>
+      <c r="B14" s="0" t="str">
+        <v>pjesuss120@gmail.com</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <v>2022-12-10 00:00:00 UTC</v>
+      </c>
+      <c r="D14" s="0" t="str">
+        <v>2022-12-15 00:00:00 UTC</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>